<commit_message>
code remis au propre
</commit_message>
<xml_diff>
--- a/Doc/Journal de travail.xlsx
+++ b/Doc/Journal de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timothee\CLionProjects\Bataille-navale\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C79F75-B4A3-46D4-9472-20890E1902AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105FFC8A-BF96-429B-A6F5-9495D5F8583E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{5CD79DA9-5221-4172-963D-ED5E747AE188}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="107">
   <si>
     <t>Date</t>
   </si>
@@ -352,6 +352,12 @@
   </si>
   <si>
     <t>mettre les fichiers externes dans des sous dossiers</t>
+  </si>
+  <si>
+    <t>nouvelles maps (5 -12)</t>
+  </si>
+  <si>
+    <t>Nettoyage du code (commentaires et fonctions)</t>
   </si>
 </sst>
 </file>
@@ -788,11 +794,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE54EA1-5D7B-45ED-AEBE-57CEB38716ED}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2379,11 +2385,13 @@
       <c r="C54" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D54" s="6"/>
+      <c r="D54" s="6">
+        <v>0.63194444444444442</v>
+      </c>
       <c r="E54" s="6"/>
-      <c r="F54" s="6" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+      <c r="F54" s="6">
+        <f t="shared" si="2"/>
+        <v>4.8611111111111049E-2</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>14</v>
@@ -2397,19 +2405,77 @@
       <c r="J54" s="9"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
+      <c r="A55" s="4">
+        <v>43928</v>
+      </c>
+      <c r="B55" s="11">
+        <v>7</v>
+      </c>
+      <c r="C55" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="D55" s="6">
+        <v>0.65277777777777779</v>
+      </c>
       <c r="E55" s="6"/>
-      <c r="F55" s="6" t="str">
-        <f t="shared" si="2"/>
+      <c r="F55" s="6">
+        <f t="shared" ref="F55:F56" si="3">IF(AND(C55&lt;&gt;"",D55&lt;&gt;""),D55-C55-E55,"")</f>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="J55" s="9"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>43928</v>
+      </c>
+      <c r="B56" s="11">
+        <v>7</v>
+      </c>
+      <c r="C56" s="6">
+        <v>0.65625</v>
+      </c>
+      <c r="D56" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6">
+        <f t="shared" ref="F56:F57" si="4">IF(AND(C56&lt;&gt;"",D56&lt;&gt;""),D56-C56-E56,"")</f>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="J56" s="9"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="G55" s="5"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2422,7 +2488,7 @@
           <x14:formula1>
             <xm:f>listes!$2:$2</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G55</xm:sqref>
+          <xm:sqref>G2:G57</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>